<commit_message>
added "Thank you" screen. updated questions and questionnaire functions.
</commit_message>
<xml_diff>
--- a/convertExcel/funfacts.xlsx
+++ b/convertExcel/funfacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\FacultyGamePhaser\convertExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DC0094-C83C-40EF-B511-3416DA635250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F9891E-F084-4845-9E83-F6918C893FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="14400" windowHeight="8722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="english" sheetId="1" r:id="rId1"/>
@@ -439,9 +439,6 @@
     <t>Every healthy human heart beats more than 100,000 times a day!</t>
   </si>
   <si>
-    <t>40% of McDonalds entire profit comes from the sale of Happy Meals.</t>
-  </si>
-  <si>
     <t>Arabic numbers are actually not Arabic; the numbers were invented in fact in India.</t>
   </si>
   <si>
@@ -655,15 +652,6 @@
     <t>The oldest evidence of manmade fire dates back 300,000 to 400,000 years. \nRecently archeologists discovered traces of campfires from 1 million years ago.</t>
   </si>
   <si>
-    <t>For over 30 years, Canada and Denmark have been fighting for control of Hans Island near Greenland.\n When officials from each country visit, \nthey leave a bottle of their country’s liquor as a power move.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The British Empire is the largest empire in worlds history.\n The British Empire was most powerful in the 1920s when it ruled over 23 percent of the world’s population. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Eiffel Tower was built from 1887 to 1889 by French engineer Gustave Eiffel.\n The tower was later named after Mr. Eiffel. </t>
-  </si>
-  <si>
     <t>From 1912 to 1948, the Olympic Games held competitions in the fine arts. \nMedals were given for literature, architecture, sculpture, painting, and music.</t>
   </si>
   <si>
@@ -676,9 +664,6 @@
     <t>The song Baby Shark is YouTube’s most viewed video ever.\n It has been viewed more than 7 billion times since its release in 2016.</t>
   </si>
   <si>
-    <t>The first email was sent as early as 1971.\n The sender, Ray Tomilinson,was the inventor of email and he sent the email to himself.</t>
-  </si>
-  <si>
     <t>The internet weighs as much as a strawberry.\n That is the weight of billions of electrons of data in motion on the web.</t>
   </si>
   <si>
@@ -712,18 +697,9 @@
     <t xml:space="preserve">A report from 2019 shows that on average every person spends 6 hours\n and 42 minutes online each day. </t>
   </si>
   <si>
-    <t>In 2016 over 15 billion Internet-connected devices \nwere shipped across the globe!</t>
-  </si>
-  <si>
-    <t>The most popular use of the internet is Electronic mail.\n At least 85% of internet users send and receive e-mail. Approximately 20 million e-mails are sent every week.</t>
-  </si>
-  <si>
     <t>The first webcam video is from the University of Cambridge.\n The subject of the first live video feed was a coffee pot.</t>
   </si>
   <si>
-    <t>A smart home is a home that is connected to the internet and can be controlled by a personal device. \nThere are currently 150 million smart homes around the globe.</t>
-  </si>
-  <si>
     <t>Asia has the most internet users with more than 35% of the total number. \nEurope ranks second with around 30% and the US ranks third with around 20%.</t>
   </si>
   <si>
@@ -748,9 +724,6 @@
     <t>The dust from the Sahara Desert travels over the \nAtlantic all the way to the Amazon Forrest on the other side of the world. \nThe Rain forest needs the dust in order to flourish.</t>
   </si>
   <si>
-    <t>A new type of stone has been discovered in the ocean. \nThe stone was created from stray plastic.</t>
-  </si>
-  <si>
     <t>Organic farming is not always better for the environment than conventional farming.\n This is partialy due to lower crop yields and the use of toxic "natural" pesticides.</t>
   </si>
   <si>
@@ -775,12 +748,6 @@
     <t>In 2015, a Canadian astronaut named Chris Hadfield released his first album,\n which was entirely recorded while he was in outer space.</t>
   </si>
   <si>
-    <t>A study from 2013 shows that music Helps People \nwith Brain Injuries Recall Personal Memories.</t>
-  </si>
-  <si>
-    <t>The life expectancy of an artist is 25 years lower than average. \nThat's because many musicians suffer from depression and lead a rough life.</t>
-  </si>
-  <si>
     <t>Plants can grow faster when they listen to music. \nResearch shows that plants particularly appreciate Beethoven and Chopin.</t>
   </si>
   <si>
@@ -790,15 +757,9 @@
     <t>Termites love rock music, according to Australian researchers\n they eat the wood twice as fast when exposed to Heavy Metal music.</t>
   </si>
   <si>
-    <t>In 2008, researchers discovered that loud \nmusic makes people drink faster.</t>
-  </si>
-  <si>
     <t>Mozart has a chocolate brand named after him called \nMozartkugel or Mozart ball. The chocolate is very popular in Austria.</t>
   </si>
   <si>
-    <t>Research shows that babies become twice as calm from listening to music as from listening to a voice. \nThey especially prefer quiet music such as children's songs, \nclassical music and smooth jazz.</t>
-  </si>
-  <si>
     <t>Eminem’s song “Rap God” has the world record for most \nwords in a song, at 1,560 words. An average of 4.28 words per second.</t>
   </si>
   <si>
@@ -817,15 +778,9 @@
     <t>The first living creature in space was a dog named Laika.\n She was taken from the street by Russians and sent to space with the Sputnik 2.</t>
   </si>
   <si>
-    <t xml:space="preserve">Theories suggest that when Earth was a relatively young planet,\n it was struck by a giant object and this collision broke a piece of the Earth away to create the moon. </t>
-  </si>
-  <si>
     <t>For years, Earth was believed to be the only planet in our\n solar system with liquid water. Recently, NASA revealed that there is \noccasional running water on Mars!</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks to 3D printing, NASA can basically “email” tools to astronauts.\n The necessary tools are designed and sent to the 3D printers to be printed in space. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> The difference between an asteroid and a comet is the composition. \nAsteroides are usually made of stone and metal, while comets also contain ice,\n particulate matter and organic matter.</t>
   </si>
   <si>
@@ -838,9 +793,6 @@
     <t>80,000 hours of video footage is uploaded to YouTube every day.\n Most of the footage is videos of pets.</t>
   </si>
   <si>
-    <t>One in ten young people was bullied on the internet last year. \nThey were victims of slander, stalking, threats and blackmail.</t>
-  </si>
-  <si>
     <t>The most common form of cyberbullying is slander.\n Slander is the use of hurtful texts or distributing photos and videos.</t>
   </si>
   <si>
@@ -878,9 +830,6 @@
   </si>
   <si>
     <t>Farm-raised salmon have a different diet then wild salmon so \nthey end up being white instead of pink. The farm raised salmon is then dyed\n pink so it’s more appealing to buyers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expiration dates on bottled water have nothing to do with the water. \nThe expiration date is for the bottle that the water is in. n. </t>
   </si>
   <si>
     <t>If you need to test the freshness of your eggs, put them in a glass of cold water.\n The fresher the egg, the faster it will fall to the bottom! \nAny eggs that float should be thrown out.</t>
@@ -1002,6 +951,57 @@
   </si>
   <si>
     <t>The human brain is made up of approximately 75% water.</t>
+  </si>
+  <si>
+    <t>The Eiffel Tower was built from 1887 to 1889 by French engineer Gustave Eiffel.\n The tower was later named after him.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The British Empire is the largest empire in worlds history.\n The British Empire was most powerful in the 1920s when it ruled over 23 \npercent of the world’s population. </t>
+  </si>
+  <si>
+    <t>For over 30 years, Canada and Denmark have been \nfighting for control of Hans Island near Greenland. When officials from each country visit, \nthey leave a bottle of their country’s liquor as a power move.</t>
+  </si>
+  <si>
+    <t>The first email was sent as early as 1971.\n The sender, Ray Tomilinson, was the inventor of email and he sent the email to himself.</t>
+  </si>
+  <si>
+    <t>In 2016 over 15 billion Internet-connected devices were shipped across the globe!</t>
+  </si>
+  <si>
+    <t>The most popular use of the internet is Electronic mail.\n At least 85% of internet users send and receive e-mail. \nApproximately 20 million e-mails are sent every week.</t>
+  </si>
+  <si>
+    <t>A smart home is a home that is connected to the internet\n and can be controlled by a personal device. There are currently\n 150 million smart homes around the globe.</t>
+  </si>
+  <si>
+    <t>A new type of stone has been discovered in the ocean. \nThe stone was created from plastic waste.</t>
+  </si>
+  <si>
+    <t>Expiration dates on bottled water have nothing to do with the water. \nThe expiration date is for the bottle that the water is in.</t>
+  </si>
+  <si>
+    <t>40% of McDonalds entire profit comes from the sale of their Happy Meals.</t>
+  </si>
+  <si>
+    <t>A study from 2013 shows that music Helps People \nwith Brain Injuries Recall personal memories.</t>
+  </si>
+  <si>
+    <t>The life expectancy of an artist is 25 years lower than the average. \nThat's because many musicians suffer from depression and lead a rough life.</t>
+  </si>
+  <si>
+    <t>In 2008, researchers discovered that loud music makes people drink faster.</t>
+  </si>
+  <si>
+    <t>Research shows that babies become twice as calm from\n listening to music as from listening to a voice. They especially prefer \nquiet music such as children's songs, classical music or smooth jazz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theories suggest that when Earth was a relatively young planet,\n it was struck by a giant object and this collision broke a piece\n of the Earth away to create the moon. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks to 3D printing, NASA can basically “email” tools to astronauts.\n The necessary tools are designed and sent to the 3D printers to be printed in outer space. </t>
+  </si>
+  <si>
+    <t>One in ten young people were bullied on the internet last year. \nThey were victims of slander, stalking, threats and blackmail.</t>
   </si>
 </sst>
 </file>
@@ -1462,6 +1462,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1470,85 +1549,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1839,533 +1839,533 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="A1:Q10"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49">
+      <c r="B1" s="46">
         <v>1</v>
       </c>
-      <c r="C1" s="49">
+      <c r="C1" s="46">
         <v>2</v>
       </c>
-      <c r="D1" s="49">
+      <c r="D1" s="46">
         <v>3</v>
       </c>
-      <c r="E1" s="49">
+      <c r="E1" s="46">
         <v>4</v>
       </c>
-      <c r="F1" s="49">
+      <c r="F1" s="46">
         <v>5</v>
       </c>
-      <c r="G1" s="49">
+      <c r="G1" s="46">
         <v>6</v>
       </c>
-      <c r="H1" s="49">
+      <c r="H1" s="46">
         <v>7</v>
       </c>
-      <c r="I1" s="50">
+      <c r="I1" s="47">
         <v>8</v>
       </c>
-      <c r="J1" s="50">
+      <c r="J1" s="47">
         <v>9</v>
       </c>
-      <c r="K1" s="51">
+      <c r="K1" s="48">
         <v>10</v>
       </c>
-      <c r="L1" s="49">
+      <c r="L1" s="46">
         <v>11</v>
       </c>
-      <c r="M1" s="49">
+      <c r="M1" s="46">
         <v>12</v>
       </c>
-      <c r="N1" s="49">
+      <c r="N1" s="46">
         <v>13</v>
       </c>
-      <c r="O1" s="49">
+      <c r="O1" s="46">
         <v>14</v>
       </c>
-      <c r="P1" s="49">
+      <c r="P1" s="46">
         <v>15</v>
       </c>
       <c r="Q1" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:28" ht="285" x14ac:dyDescent="0.45">
+      <c r="A2" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="53" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>302</v>
-      </c>
-      <c r="D2" s="53" t="s">
-        <v>309</v>
-      </c>
-      <c r="E2" s="55" t="s">
+      <c r="B2" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="55" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="56" t="s">
-        <v>221</v>
-      </c>
-      <c r="G2" s="54" t="s">
+      <c r="L2" s="56" t="s">
+        <v>293</v>
+      </c>
+      <c r="M2" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="N2" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="I2" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>217</v>
-      </c>
-      <c r="K2" s="58" t="s">
-        <v>218</v>
-      </c>
-      <c r="L2" s="59" t="s">
-        <v>310</v>
-      </c>
-      <c r="M2" s="60" t="s">
-        <v>219</v>
-      </c>
-      <c r="N2" s="61" t="s">
-        <v>220</v>
-      </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="399" x14ac:dyDescent="0.45">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>292</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>311</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>312</v>
-      </c>
-      <c r="E3" s="53" t="s">
+      <c r="B3" s="52" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="G3" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="H3" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="H3" s="58" t="s">
+      <c r="I3" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="K3" s="57" t="s">
+        <v>304</v>
+      </c>
+      <c r="L3" s="57" t="s">
+        <v>303</v>
+      </c>
+      <c r="M3" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="I3" s="59" t="s">
-        <v>133</v>
-      </c>
-      <c r="J3" s="60" t="s">
+      <c r="O3" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="K3" s="60" t="s">
-        <v>205</v>
-      </c>
-      <c r="L3" s="60" t="s">
-        <v>206</v>
-      </c>
-      <c r="M3" s="64" t="s">
-        <v>134</v>
-      </c>
-      <c r="N3" s="65" t="s">
-        <v>207</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>208</v>
-      </c>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="54"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="51"/>
     </row>
     <row r="4" spans="1:28" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="53" t="s">
-        <v>294</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>209</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>313</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>210</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" s="53" t="s">
-        <v>295</v>
-      </c>
-      <c r="H4" s="55" t="s">
-        <v>212</v>
-      </c>
-      <c r="I4" s="54" t="s">
-        <v>222</v>
-      </c>
-      <c r="J4" s="54" t="s">
-        <v>223</v>
-      </c>
-      <c r="K4" s="58" t="s">
-        <v>224</v>
-      </c>
-      <c r="L4" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="M4" s="58" t="s">
-        <v>226</v>
-      </c>
-      <c r="N4" s="59" t="s">
+      <c r="B4" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>306</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>278</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>307</v>
+      </c>
+      <c r="K4" s="55" t="s">
+        <v>308</v>
+      </c>
+      <c r="L4" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="M4" s="55" t="s">
+        <v>309</v>
+      </c>
+      <c r="N4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="66" t="s">
+      <c r="O4" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="65" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q4" s="62"/>
+      <c r="P4" s="62" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q4" s="59"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
     </row>
     <row r="5" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" s="53" t="s">
+      <c r="B5" s="51" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" s="60" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>226</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>310</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="N5" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="O5" s="62" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="P5" s="62" t="s">
         <v>231</v>
       </c>
-      <c r="G5" s="58" t="s">
-        <v>232</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>233</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>314</v>
-      </c>
-      <c r="J5" s="58" t="s">
-        <v>234</v>
-      </c>
-      <c r="K5" s="57" t="s">
-        <v>235</v>
-      </c>
-      <c r="L5" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="M5" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="N5" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="O5" s="65" t="s">
-        <v>239</v>
-      </c>
-      <c r="P5" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q5" s="62"/>
+      <c r="Q5" s="59"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="384.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="52" t="s">
+    <row r="6" spans="1:28" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>313</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>235</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="K6" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="C6" s="53" t="s">
-        <v>241</v>
-      </c>
-      <c r="D6" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>244</v>
-      </c>
-      <c r="G6" s="53" t="s">
-        <v>245</v>
-      </c>
-      <c r="H6" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="I6" s="54" t="s">
-        <v>247</v>
-      </c>
-      <c r="J6" s="54" t="s">
-        <v>248</v>
-      </c>
-      <c r="K6" s="54" t="s">
-        <v>249</v>
-      </c>
-      <c r="L6" s="54" t="s">
-        <v>250</v>
-      </c>
-      <c r="M6" s="67" t="s">
-        <v>251</v>
-      </c>
-      <c r="N6" s="65" t="s">
-        <v>252</v>
-      </c>
-      <c r="O6" s="64" t="s">
-        <v>253</v>
-      </c>
-      <c r="P6" s="65" t="s">
+      <c r="L6" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="M6" s="64" t="s">
+        <v>316</v>
+      </c>
+      <c r="N6" s="62" t="s">
+        <v>239</v>
+      </c>
+      <c r="O6" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="P6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="62"/>
+      <c r="Q6" s="59"/>
       <c r="AA6" s="5"/>
     </row>
     <row r="7" spans="1:28" ht="370.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>307</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>254</v>
-      </c>
-      <c r="E7" s="53" t="s">
+      <c r="B7" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="I7" s="65" t="s">
+        <v>287</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="K7" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="L7" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="M7" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="53" t="s">
-        <v>255</v>
-      </c>
-      <c r="G7" s="54" t="s">
-        <v>256</v>
-      </c>
-      <c r="H7" s="55" t="s">
-        <v>257</v>
-      </c>
-      <c r="I7" s="68" t="s">
-        <v>304</v>
-      </c>
-      <c r="J7" s="54" t="s">
-        <v>258</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>259</v>
-      </c>
-      <c r="L7" s="58" t="s">
-        <v>260</v>
-      </c>
-      <c r="M7" s="57" t="s">
-        <v>136</v>
-      </c>
-      <c r="N7" s="59" t="s">
-        <v>261</v>
-      </c>
-      <c r="O7" s="59" t="s">
-        <v>262</v>
-      </c>
-      <c r="P7" s="60" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q7" s="62"/>
+      <c r="N7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="O7" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="P7" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q7" s="59"/>
       <c r="Y7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
     </row>
     <row r="8" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>308</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>316</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>306</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>317</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>264</v>
-      </c>
-      <c r="H8" s="55" t="s">
-        <v>265</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>266</v>
-      </c>
-      <c r="J8" s="54" t="s">
-        <v>267</v>
-      </c>
-      <c r="K8" s="54" t="s">
-        <v>268</v>
-      </c>
-      <c r="L8" s="54" t="s">
-        <v>269</v>
-      </c>
-      <c r="M8" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="N8" s="60" t="s">
-        <v>271</v>
-      </c>
-      <c r="O8" s="65" t="s">
-        <v>272</v>
-      </c>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
+      <c r="B8" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>319</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="M8" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="N8" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="O8" s="62" t="s">
+        <v>256</v>
+      </c>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
       <c r="AB8" s="5"/>
     </row>
     <row r="9" spans="1:28" ht="384.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="53" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9" s="53" t="s">
+      <c r="B9" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="E9" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="53" t="s">
-        <v>276</v>
-      </c>
-      <c r="G9" s="54" t="s">
-        <v>277</v>
-      </c>
-      <c r="H9" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="I9" s="69" t="s">
-        <v>297</v>
-      </c>
-      <c r="J9" s="54" t="s">
-        <v>279</v>
-      </c>
-      <c r="K9" s="57" t="s">
+      <c r="F9" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="G9" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="I9" s="66" t="s">
+        <v>280</v>
+      </c>
+      <c r="J9" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="K9" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="57" t="s">
-        <v>132</v>
-      </c>
-      <c r="M9" s="58" t="s">
-        <v>280</v>
-      </c>
-      <c r="N9" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="O9" s="65" t="s">
-        <v>282</v>
-      </c>
-      <c r="P9" s="65" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q9" s="64" t="s">
+      <c r="L9" s="54" t="s">
+        <v>312</v>
+      </c>
+      <c r="M9" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="N9" s="67" t="s">
+        <v>264</v>
+      </c>
+      <c r="O9" s="62" t="s">
+        <v>265</v>
+      </c>
+      <c r="P9" s="62" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q9" s="61" t="s">
         <v>6</v>
       </c>
       <c r="AB9" s="5"/>
     </row>
     <row r="10" spans="1:28" ht="285" x14ac:dyDescent="0.45">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>282</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>269</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="I10" s="54" t="s">
         <v>284</v>
       </c>
-      <c r="C10" s="53" t="s">
-        <v>298</v>
-      </c>
-      <c r="D10" s="54" t="s">
-        <v>285</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>286</v>
-      </c>
-      <c r="G10" s="53" t="s">
-        <v>287</v>
-      </c>
-      <c r="H10" s="56" t="s">
-        <v>300</v>
-      </c>
-      <c r="I10" s="57" t="s">
+      <c r="J10" s="54" t="s">
+        <v>271</v>
+      </c>
+      <c r="K10" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="68" t="s">
+        <v>272</v>
+      </c>
+      <c r="M10" s="69" t="s">
         <v>301</v>
       </c>
-      <c r="J10" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="K10" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" s="71" t="s">
-        <v>289</v>
-      </c>
-      <c r="M10" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="N10" s="58" t="s">
-        <v>290</v>
-      </c>
-      <c r="O10" s="59" t="s">
-        <v>319</v>
-      </c>
-      <c r="P10" s="73" t="s">
+      <c r="N10" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="O10" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="P10" s="70" t="s">
         <v>131</v>
       </c>
-      <c r="Q10" s="74" t="s">
-        <v>291</v>
+      <c r="Q10" s="71" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2458,7 +2458,7 @@
         <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>47</v>
@@ -2467,10 +2467,10 @@
         <v>54</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>76</v>
@@ -2479,7 +2479,7 @@
         <v>35</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>30</v>
@@ -2488,7 +2488,7 @@
         <v>59</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R2" s="9"/>
     </row>
@@ -2500,10 +2500,10 @@
         <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>36</v>
@@ -2518,7 +2518,7 @@
         <v>65</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>22</v>
@@ -2533,13 +2533,13 @@
         <v>81</v>
       </c>
       <c r="N3" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="P3" s="29" t="s">
         <v>146</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="301.89999999999998" x14ac:dyDescent="0.45">
@@ -2550,25 +2550,25 @@
         <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>78</v>
@@ -2586,13 +2586,13 @@
         <v>71</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>57</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R4" s="8"/>
     </row>
@@ -2613,19 +2613,19 @@
         <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" s="22" t="s">
         <v>157</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>158</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>60</v>
       </c>
       <c r="I5" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="J5" s="18" t="s">
         <v>159</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>72</v>
@@ -2643,7 +2643,7 @@
         <v>48</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q5" s="32" t="s">
         <v>90</v>
@@ -2657,16 +2657,16 @@
         <v>99</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>44</v>
@@ -2675,13 +2675,13 @@
         <v>49</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>68</v>
@@ -2693,13 +2693,13 @@
         <v>58</v>
       </c>
       <c r="O6" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="P6" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="Q6" s="32" t="s">
         <v>169</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="242.25" x14ac:dyDescent="0.45">
@@ -2713,7 +2713,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>79</v>
@@ -2722,19 +2722,19 @@
         <v>38</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>85</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>63</v>
@@ -2746,7 +2746,7 @@
         <v>32</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P7" s="16" t="s">
         <v>50</v>
@@ -2763,10 +2763,10 @@
         <v>101</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>33</v>
@@ -2775,34 +2775,34 @@
         <v>39</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>92</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>75</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O8" s="14" t="s">
         <v>61</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="275.64999999999998" x14ac:dyDescent="0.45">
@@ -2816,10 +2816,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>40</v>
@@ -2834,28 +2834,28 @@
         <v>87</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>28</v>
       </c>
       <c r="M9" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="N9" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="O9" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="P9" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="P9" s="28" t="s">
+      <c r="Q9" s="28" t="s">
         <v>192</v>
-      </c>
-      <c r="Q9" s="28" t="s">
-        <v>193</v>
       </c>
       <c r="R9" s="28" t="s">
         <v>52</v>
@@ -2869,16 +2869,16 @@
         <v>102</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>93</v>
@@ -2887,7 +2887,7 @@
         <v>53</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>34</v>
@@ -2899,10 +2899,10 @@
         <v>64</v>
       </c>
       <c r="M10" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="N10" s="21" t="s">
         <v>198</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>199</v>
       </c>
       <c r="O10" s="21" t="s">
         <v>94</v>
@@ -2950,16 +2950,16 @@
       <c r="C1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="47"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
hebrew assets + questionnaire
</commit_message>
<xml_diff>
--- a/convertExcel/funfacts.xlsx
+++ b/convertExcel/funfacts.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\FacultyGamePhaser\convertExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49D1FE4-FE68-4970-8792-0D4FF1EA4839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0AEDF8-0653-4D00-B838-2E34EBBED763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="english" sheetId="1" r:id="rId1"/>
     <sheet name="hebrew" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="removedFacts" sheetId="2" r:id="rId4"/>
+    <sheet name="removedFacts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="320">
   <si>
     <t>category</t>
   </si>
@@ -467,9 +466,6 @@
     <t xml:space="preserve">חסילון הוא החיה הרועשת בעולם וגבהה רק שני ס"מ! הצליל שהחסילון משמיע כשהוא מקיש בצבתותיו עולה על 218 דציבלים וחזק יותר מרעש של אקדח. </t>
   </si>
   <si>
-    <t>אלברט איינשטיין היה יהודי. אמנם לא היה אזרח ישראלי, אך בשנת 1952 הוצע לו להיות ראש ממשלת ישראל וסירב.</t>
-  </si>
-  <si>
     <t>האפיפיור בנדיקט התשיעי היה האפיפיור הצעיר ביותר בעולם בגיל 11. הוא שירת כאפיפיור בין השנים 1032 ל1048.</t>
   </si>
   <si>
@@ -488,9 +484,6 @@
     <t>כ204 מיליון אימיילים נשלחים כל דקה באינטרנט. 70% מהאימיילים הנשלחים הם ספאם.</t>
   </si>
   <si>
-    <t xml:space="preserve">גוגל מעבד עד 100 ביליון חיפושים בחודש! כלומר בכל שניה מתבצעים בממוצע 40,000 חיפושים. </t>
-  </si>
-  <si>
     <t>עד 300,000 אתרי אינטרנט נפרצים בכל יום. פושעי סייבר נעזרים בתוכנות מחשב משוכללות לפרוץ באופן אוטומטי לאתרים פגיעים.</t>
   </si>
   <si>
@@ -621,9 +614,6 @@
   </si>
   <si>
     <t>מנהג הרמת כוס  התחילה בתקופת הרומאים. באותה תקופה, נהגו רומאים רבים להרעיל זה את זה. בהרמת כוס בעוצמה רבה - חלק מהמשקה מועבר מכוס לכוס וכך השותה מוודא שמשקעו לא הורעל.</t>
-  </si>
-  <si>
-    <t>תינוקות נולדים ללא ברכיים. הן לא מופיעות עד שהילד בין שנתיים ל-6 שנים.</t>
   </si>
   <si>
     <t xml:space="preserve">המוח הוא איבר מקומט מאוד! אם פורשים אותו, המוח יהיה בערך בגודל ציפית של כרית. </t>
@@ -1005,7 +995,13 @@
     <t>One in ten young people were bullied on the internet last year. \nThey were victims of slander, stalking, threats and blackmail.</t>
   </si>
   <si>
-    <t xml:space="preserve">לירח אין אטמוספירה, לכן אין אוויר שישחק את האדמה ואין מים שישטפו את הקרקע. מכאן שעקבות אסטרונאוטים יישארו על ירח לאלפי שנים. </t>
+    <t>תינוקות נולדים ללא פיקת ברכיים. הן לא מופיעות עד שהילד בין שנתיים ל-6 שנים.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">גוגל מעבדת עד 100 מיליארד חיפושים בחודש! כלומר בכל שניה מתבצעים בממוצע 40,000 חיפושים. </t>
+  </si>
+  <si>
+    <t>אלברט איינשטיין היה יהודי. 9987 אמנם לא היה אזרח ישראלי, אך בשנת 1952 הוצע לו להיות ראש ממשלת ישראל וסירב.</t>
   </si>
 </sst>
 </file>
@@ -1340,99 +1336,11 @@
   </cellStyleXfs>
   <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1553,6 +1461,96 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1852,524 +1850,524 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46">
+      <c r="B1" s="16">
         <v>1</v>
       </c>
-      <c r="C1" s="46">
+      <c r="C1" s="16">
         <v>2</v>
       </c>
-      <c r="D1" s="46">
+      <c r="D1" s="16">
         <v>3</v>
       </c>
-      <c r="E1" s="46">
+      <c r="E1" s="16">
         <v>4</v>
       </c>
-      <c r="F1" s="46">
+      <c r="F1" s="16">
         <v>5</v>
       </c>
-      <c r="G1" s="46">
+      <c r="G1" s="16">
         <v>6</v>
       </c>
-      <c r="H1" s="46">
+      <c r="H1" s="16">
         <v>7</v>
       </c>
-      <c r="I1" s="47">
+      <c r="I1" s="17">
         <v>8</v>
       </c>
-      <c r="J1" s="47">
+      <c r="J1" s="17">
         <v>9</v>
       </c>
-      <c r="K1" s="48">
+      <c r="K1" s="18">
         <v>10</v>
       </c>
-      <c r="L1" s="46">
+      <c r="L1" s="16">
         <v>11</v>
       </c>
-      <c r="M1" s="46">
+      <c r="M1" s="16">
         <v>12</v>
       </c>
-      <c r="N1" s="46">
+      <c r="N1" s="16">
         <v>13</v>
       </c>
-      <c r="O1" s="46">
+      <c r="O1" s="16">
         <v>14</v>
       </c>
-      <c r="P1" s="46">
+      <c r="P1" s="16">
         <v>15</v>
       </c>
-      <c r="Q1" s="6">
+      <c r="Q1" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="285" x14ac:dyDescent="0.45">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+    </row>
+    <row r="3" spans="1:28" ht="399" x14ac:dyDescent="0.45">
+      <c r="A3" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>285</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>292</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>208</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="H2" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="J2" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="K2" s="55" t="s">
-        <v>213</v>
-      </c>
-      <c r="L2" s="56" t="s">
-        <v>293</v>
-      </c>
-      <c r="M2" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="N2" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-    </row>
-    <row r="3" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>275</v>
-      </c>
-      <c r="C3" s="50" t="s">
-        <v>294</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>295</v>
-      </c>
-      <c r="E3" s="50" t="s">
+      <c r="I3" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="O3" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="H3" s="55" t="s">
-        <v>202</v>
-      </c>
-      <c r="I3" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="K3" s="57" t="s">
-        <v>304</v>
-      </c>
-      <c r="L3" s="57" t="s">
-        <v>303</v>
-      </c>
-      <c r="M3" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="N3" s="62" t="s">
-        <v>203</v>
-      </c>
-      <c r="O3" s="61" t="s">
-        <v>204</v>
-      </c>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="51"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="21"/>
     </row>
     <row r="4" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="F4" s="50" t="s">
+      <c r="B4" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="M4" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="G4" s="50" t="s">
-        <v>278</v>
-      </c>
-      <c r="H4" s="52" t="s">
-        <v>207</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>307</v>
-      </c>
-      <c r="K4" s="55" t="s">
-        <v>308</v>
-      </c>
-      <c r="L4" s="55" t="s">
-        <v>218</v>
-      </c>
-      <c r="M4" s="55" t="s">
-        <v>309</v>
-      </c>
-      <c r="N4" s="56" t="s">
+      <c r="N4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="63" t="s">
+      <c r="O4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="62" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q4" s="59"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
+      <c r="P4" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q4" s="29"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:28" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>279</v>
-      </c>
-      <c r="C5" s="50" t="s">
+      <c r="B5" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="G5" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="H5" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="I5" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="J5" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="K5" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="L5" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="H5" s="55" t="s">
+      <c r="M5" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="I5" s="55" t="s">
-        <v>297</v>
-      </c>
-      <c r="J5" s="55" t="s">
+      <c r="N5" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="O5" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q5" s="29"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="L5" s="54" t="s">
-        <v>227</v>
-      </c>
-      <c r="M5" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="N5" s="56" t="s">
-        <v>229</v>
-      </c>
-      <c r="O5" s="62" t="s">
-        <v>230</v>
-      </c>
-      <c r="P5" s="62" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q5" s="59"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-    </row>
-    <row r="6" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>298</v>
-      </c>
-      <c r="C6" s="50" t="s">
+      <c r="G6" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="I6" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="J6" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="K6" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="M6" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="G6" s="50" t="s">
-        <v>314</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>235</v>
-      </c>
-      <c r="I6" s="51" t="s">
+      <c r="N6" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="O6" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="K6" s="51" t="s">
-        <v>315</v>
-      </c>
-      <c r="L6" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="M6" s="64" t="s">
-        <v>316</v>
-      </c>
-      <c r="N6" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="O6" s="61" t="s">
-        <v>240</v>
-      </c>
-      <c r="P6" s="62" t="s">
+      <c r="P6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="59"/>
-      <c r="AA6" s="5"/>
+      <c r="Q6" s="29"/>
+      <c r="AA6" s="1"/>
     </row>
     <row r="7" spans="1:28" ht="370.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7" s="51" t="s">
+      <c r="B7" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="H7" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="E7" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="50" t="s">
+      <c r="I7" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="K7" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="G7" s="51" t="s">
+      <c r="L7" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="O7" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="I7" s="65" t="s">
-        <v>287</v>
-      </c>
-      <c r="J7" s="51" t="s">
-        <v>317</v>
-      </c>
-      <c r="K7" s="55" t="s">
+      <c r="P7" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="L7" s="55" t="s">
-        <v>318</v>
-      </c>
-      <c r="M7" s="54" t="s">
-        <v>135</v>
-      </c>
-      <c r="N7" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="O7" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="P7" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q7" s="59"/>
-      <c r="Y7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
+      <c r="Q7" s="29"/>
+      <c r="Y7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="50" t="s">
-        <v>291</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="50" t="s">
+      <c r="B8" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="E8" s="50" t="s">
-        <v>289</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="G8" s="50" t="s">
+      <c r="C8" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="H8" s="52" t="s">
-        <v>319</v>
-      </c>
-      <c r="I8" s="53" t="s">
+      <c r="L8" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="M8" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="K8" s="51" t="s">
+      <c r="N8" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="L8" s="51" t="s">
+      <c r="O8" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="M8" s="51" t="s">
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A9" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="N8" s="57" t="s">
+      <c r="C9" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="O8" s="62" t="s">
+      <c r="D9" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="AB8" s="5"/>
-    </row>
-    <row r="9" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="50" t="s">
+      <c r="E9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="G9" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="H9" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="50" t="s">
+      <c r="I9" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="M9" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="G9" s="51" t="s">
+      <c r="N9" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="H9" s="51" t="s">
+      <c r="O9" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="I9" s="66" t="s">
-        <v>280</v>
-      </c>
-      <c r="J9" s="51" t="s">
-        <v>311</v>
-      </c>
-      <c r="K9" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="54" t="s">
-        <v>312</v>
-      </c>
-      <c r="M9" s="55" t="s">
+      <c r="P9" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="N9" s="67" t="s">
-        <v>264</v>
-      </c>
-      <c r="O9" s="62" t="s">
-        <v>265</v>
-      </c>
-      <c r="P9" s="62" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q9" s="61" t="s">
+      <c r="Q9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="AB9" s="5"/>
+      <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:28" ht="285" x14ac:dyDescent="0.45">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="H10" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="I10" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="J10" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="51" t="s">
-        <v>282</v>
-      </c>
-      <c r="F10" s="51" t="s">
+      <c r="K10" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="M10" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="N10" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="H10" s="53" t="s">
-        <v>283</v>
-      </c>
-      <c r="I10" s="54" t="s">
-        <v>284</v>
-      </c>
-      <c r="J10" s="54" t="s">
+      <c r="O10" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="P10" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q10" s="41" t="s">
         <v>271</v>
-      </c>
-      <c r="K10" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="L10" s="68" t="s">
-        <v>272</v>
-      </c>
-      <c r="M10" s="69" t="s">
-        <v>301</v>
-      </c>
-      <c r="N10" s="55" t="s">
-        <v>273</v>
-      </c>
-      <c r="O10" s="56" t="s">
-        <v>302</v>
-      </c>
-      <c r="P10" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q10" s="71" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2383,541 +2381,550 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449B4987-24CE-40C9-AE43-0C2DF0653AF4}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K9" sqref="A1:R10"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:18" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="46">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="46">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="46">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="46">
         <v>4</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="46">
         <v>5</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="46">
         <v>6</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="46">
         <v>7</v>
       </c>
-      <c r="J1" s="10">
+      <c r="J1" s="47">
         <v>8</v>
       </c>
-      <c r="K1" s="10">
+      <c r="K1" s="47">
         <v>9</v>
       </c>
-      <c r="L1" s="10">
+      <c r="L1" s="47">
         <v>10</v>
       </c>
-      <c r="M1" s="10">
+      <c r="M1" s="47">
         <v>11</v>
       </c>
-      <c r="N1" s="10">
+      <c r="N1" s="47">
         <v>12</v>
       </c>
-      <c r="O1" s="10">
+      <c r="O1" s="47">
         <v>13</v>
       </c>
-      <c r="P1" s="10">
+      <c r="P1" s="47">
         <v>14</v>
       </c>
-      <c r="Q1" s="10">
+      <c r="Q1" s="47">
         <v>15</v>
       </c>
-      <c r="R1" s="10">
+      <c r="R1" s="47">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="236.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="55" t="s">
         <v>140</v>
       </c>
-      <c r="R2" s="9"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="57"/>
     </row>
     <row r="3" spans="1:18" ht="288.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="50" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="30" t="s">
+      <c r="O3" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="P3" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="P3" s="29" t="s">
-        <v>146</v>
-      </c>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
     </row>
     <row r="4" spans="1:18" ht="301.89999999999998" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="P4" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="R4" s="8"/>
+      <c r="R4" s="64"/>
     </row>
     <row r="5" spans="1:18" ht="255" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="J5" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="23" t="s">
+      <c r="K5" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="68" t="s">
         <v>90</v>
       </c>
+      <c r="R5" s="56"/>
     </row>
     <row r="6" spans="1:18" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="G6" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="69" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="J6" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="K6" s="69" t="s">
         <v>164</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="L6" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="N6" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="P6" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="L6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" s="32" t="s">
+      <c r="Q6" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="P6" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>169</v>
-      </c>
+      <c r="R6" s="56"/>
     </row>
     <row r="7" spans="1:18" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="69" t="s">
         <v>170</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="J7" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="69" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="L7" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="17" t="s">
+      <c r="Q7" s="72" t="s">
         <v>91</v>
       </c>
+      <c r="R7" s="56"/>
     </row>
     <row r="8" spans="1:18" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="H8" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="J8" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="K8" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="M8" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="O8" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="68" t="s">
         <v>181</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="32" t="s">
-        <v>183</v>
-      </c>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
     </row>
     <row r="9" spans="1:18" ht="275.64999999999998" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="K9" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="L9" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="73" t="s">
         <v>186</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="N9" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="25" t="s">
+      <c r="O9" s="54" t="s">
         <v>188</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="P9" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="Q9" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="P9" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q9" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="R9" s="28" t="s">
+      <c r="R9" s="55" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="216.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="69" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="J10" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="N10" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="M10" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="P10" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="R10" s="15" t="s">
+      <c r="R10" s="62" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2928,566 +2935,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52965FE2-7753-40B8-A5CB-114A733C17A5}">
-  <dimension ref="A29:J46"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="29" spans="1:10" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="183.75" x14ac:dyDescent="0.45">
-      <c r="A31" s="2">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="204" x14ac:dyDescent="0.45">
-      <c r="A32" s="2">
-        <v>2</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="236.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="2">
-        <v>3</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="210" x14ac:dyDescent="0.45">
-      <c r="A34" s="2">
-        <v>4</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="216.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="2">
-        <v>5</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="204" x14ac:dyDescent="0.45">
-      <c r="A36" s="2">
-        <v>6</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="223.15" x14ac:dyDescent="0.45">
-      <c r="A37" s="2">
-        <v>7</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="236.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="10">
-        <v>8</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="J38" s="25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="236.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="10">
-        <v>9</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="288.75" x14ac:dyDescent="0.45">
-      <c r="A40" s="10">
-        <v>10</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="I40" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J40" s="26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="10">
-        <v>11</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I41" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="J41" s="27" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="10">
-        <v>12</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="242.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="10">
-        <v>13</v>
-      </c>
-      <c r="B43" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="J43" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="275.64999999999998" x14ac:dyDescent="0.45">
-      <c r="A44" s="10">
-        <v>14</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="I44" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="301.89999999999998" x14ac:dyDescent="0.45">
-      <c r="A45" s="10">
-        <v>15</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="I45" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="78.75" x14ac:dyDescent="0.45">
-      <c r="A46" s="10">
-        <v>16</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="D46" s="8"/>
-      <c r="I46" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C0FF40-061A-4942-A5B8-C1DE892A3174}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -3500,112 +2947,112 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="41"/>
-    <col min="3" max="3" width="9.06640625" style="40"/>
+    <col min="1" max="1" width="9.06640625" style="11"/>
+    <col min="3" max="3" width="9.06640625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
@@ -3614,40 +3061,40 @@
       <c r="F4" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="K4" s="44" t="s">
+      <c r="K4" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="36"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
questionnaire- added requirement to answer every question
</commit_message>
<xml_diff>
--- a/convertExcel/funfacts.xlsx
+++ b/convertExcel/funfacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\FacultyGamePhaser\convertExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0AEDF8-0653-4D00-B838-2E34EBBED763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C360B-95A7-44C1-A345-5BC1C4DE351A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,7 +1001,7 @@
     <t xml:space="preserve">גוגל מעבדת עד 100 מיליארד חיפושים בחודש! כלומר בכל שניה מתבצעים בממוצע 40,000 חיפושים. </t>
   </si>
   <si>
-    <t>אלברט איינשטיין היה יהודי. 9987 אמנם לא היה אזרח ישראלי, אך בשנת 1952 הוצע לו להיות ראש ממשלת ישראל וסירב.</t>
+    <t>אלברט איינשטיין היה יהודי. \n אמנם לא היה אזרח ישראלי, אך בשנת 1952 הוצע לו להיות ראש ממשלת ישראל וסירב.</t>
   </si>
 </sst>
 </file>
@@ -1463,94 +1463,94 @@
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment readingOrder="1"/>
+      <alignment readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
+      <alignment readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1902,7 +1902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="285" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>96</v>
       </c>
@@ -1949,7 +1949,7 @@
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
     </row>
-    <row r="3" spans="1:28" ht="399" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>97</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="370.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>99</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="Q8" s="29"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" ht="384.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" ht="356.25" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>103</v>
       </c>

</xml_diff>